<commit_message>
modify on my laptop
</commit_message>
<xml_diff>
--- a/新FW650配料系统测试20190704.xlsx
+++ b/新FW650配料系统测试20190704.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\FW650_NEW\FW650\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFEF266-F81D-4720-8CB8-0C1403C10F00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24795" windowHeight="11880"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,15 +446,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.更新屏幕程序</t>
+    <t>5.更新屏幕程序，U盘更新</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +589,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -603,14 +617,20 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="D:\Users\Documents\Tencent Files\MobileFile\Image\F$QS81[VF@%QOQ~YT9AP_`4.png"/>
+        <xdr:cNvPr id="2" name="图片 1" descr="D:\Users\Documents\Tencent Files\MobileFile\Image\F$QS81[VF@%QOQ~YT9AP_`4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -650,7 +670,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -690,14 +716,20 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3" descr="D:\Users\Documents\Tencent Files\MobileFile\Image\W@_T7L@~Y[VQLF7}_{L15RS.png"/>
+        <xdr:cNvPr id="4" name="图片 3" descr="D:\Users\Documents\Tencent Files\MobileFile\Image\W@_T7L@~Y[VQLF7}_{L15RS.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -726,7 +758,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -768,7 +800,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,9 +832,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,6 +884,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1009,25 +1077,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E25" sqref="E25:F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="58.125" customWidth="1"/>
-    <col min="4" max="4" width="47.375" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="58.109375" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -1039,7 +1107,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="20.25">
+    <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43650</v>
       </c>
@@ -1047,7 +1115,7 @@
         <v>43664</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.25" customHeight="1">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
@@ -1062,7 +1130,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="20.25">
+    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -1078,7 +1146,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" ht="20.25">
+    <row r="5" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>26</v>
@@ -1092,7 +1160,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="20.25">
+    <row r="6" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>28</v>
@@ -1106,7 +1174,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="20.25">
+    <row r="7" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>38</v>
@@ -1120,7 +1188,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="40.5">
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -1136,7 +1204,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="20.25">
+    <row r="9" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1150,7 +1218,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="20.25">
+    <row r="10" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -1162,7 +1230,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="20.25">
+    <row r="11" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -1176,7 +1244,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="20.25">
+    <row r="12" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1260,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="20.25">
+    <row r="13" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>15</v>
@@ -1206,7 +1274,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="20.25">
+    <row r="14" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>16</v>
@@ -1218,7 +1286,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="20.25">
+    <row r="15" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>17</v>
@@ -1230,7 +1298,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="20.25">
+    <row r="16" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1244,7 +1312,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="20.25">
+    <row r="17" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>21</v>
@@ -1256,7 +1324,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="20.25">
+    <row r="18" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>53</v>
@@ -1268,7 +1336,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="20.25">
+    <row r="19" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>88</v>
       </c>
@@ -1281,7 +1349,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="20.25">
+    <row r="20" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>1</v>
@@ -1293,7 +1361,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="20.25">
+    <row r="21" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
         <v>3</v>
@@ -1307,7 +1375,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="20.25">
+    <row r="22" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
         <v>4</v>
@@ -1321,7 +1389,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="20.25">
+    <row r="23" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>6</v>
@@ -1335,7 +1403,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="20.25">
+    <row r="24" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>7</v>
@@ -1349,7 +1417,7 @@
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" ht="20.25">
+    <row r="25" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>65</v>
       </c>
@@ -1365,7 +1433,7 @@
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:6" ht="20.25">
+    <row r="26" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>24</v>
@@ -1377,7 +1445,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" ht="20.25">
+    <row r="27" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>25</v>
@@ -1389,7 +1457,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="20.25">
+    <row r="28" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>29</v>
@@ -1400,7 +1468,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="20.25">
+    <row r="29" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" t="s">
         <v>31</v>
@@ -1409,7 +1477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="20.25">
+    <row r="30" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
         <v>32</v>
@@ -1418,7 +1486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="20.25">
+    <row r="31" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
         <v>33</v>
@@ -1427,7 +1495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="20.25">
+    <row r="32" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" t="s">
         <v>34</v>
@@ -1436,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20.25">
+    <row r="33" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" t="s">
         <v>35</v>
@@ -1446,7 +1514,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="20.25">
+    <row r="34" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
         <v>36</v>
@@ -1456,7 +1524,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="20.25">
+    <row r="35" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" t="s">
         <v>37</v>
@@ -1466,12 +1534,12 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="20.25">
+    <row r="36" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>43638</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="20.25">
+    <row r="37" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -1483,7 +1551,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="20.25">
+    <row r="38" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" t="s">
         <v>41</v>
@@ -1493,7 +1561,7 @@
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" ht="20.25">
+    <row r="39" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
         <v>42</v>
@@ -1503,7 +1571,7 @@
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" ht="20.25">
+    <row r="40" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" t="s">
         <v>43</v>
@@ -1513,7 +1581,7 @@
       </c>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" ht="20.25">
+    <row r="41" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1524,7 +1592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20.25">
+    <row r="42" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" t="s">
         <v>46</v>
@@ -1533,7 +1601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20.25">
+    <row r="43" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" t="s">
         <v>47</v>
@@ -1542,7 +1610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20.25">
+    <row r="44" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1554,7 +1622,7 @@
       </c>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" ht="20.25">
+    <row r="45" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
         <v>50</v>
@@ -1564,7 +1632,7 @@
       </c>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4" ht="20.25">
+    <row r="46" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" t="s">
         <v>51</v>
@@ -1574,7 +1642,7 @@
       </c>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" ht="20.25">
+    <row r="47" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" t="s">
         <v>52</v>
@@ -1584,7 +1652,7 @@
       </c>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" ht="20.25">
+    <row r="48" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -1596,7 +1664,7 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>57</v>
       </c>
@@ -1604,7 +1672,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>59</v>
       </c>
@@ -1612,7 +1680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="20.25">
+    <row r="51" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>68</v>
       </c>
@@ -1623,7 +1691,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="20.25">
+    <row r="52" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>69</v>
       </c>
@@ -1635,7 +1703,7 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>73</v>
       </c>
@@ -1643,7 +1711,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>74</v>
       </c>
@@ -1652,7 +1720,7 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>76</v>
       </c>
@@ -1660,7 +1728,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>77</v>
       </c>
@@ -1668,7 +1736,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>78</v>
       </c>
@@ -1678,20 +1746,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="D21:D27"/>
@@ -1708,6 +1762,20 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1717,12 +1785,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1730,12 +1798,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>